<commit_message>
Code updation on orderconfirmation and receipt voucher test page
</commit_message>
<xml_diff>
--- a/DCPLProjectSales/src/test/resources/TestData/TestData.xlsx
+++ b/DCPLProjectSales/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\DCPLProject\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectSales\DCPLProjectSales\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9D56A8-928C-4BE2-BF41-A5574B770672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E2598D-705B-4CB4-9308-437A6B188ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesLogin" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
   <si>
     <t>hrms_id</t>
   </si>
@@ -419,9 +419,6 @@
     <t>Axis Bank</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
     <t>2023</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
     <t>salesexecutive</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -564,6 +558,9 @@
   </si>
   <si>
     <t>28</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D04161-DFF8-4095-A5EB-FA021B973EF1}">
   <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,52 +1698,52 @@
         <v>126</v>
       </c>
       <c r="BA1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="BB1" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="BC1" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BD1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BE1" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="BE1" s="16" t="s">
+      <c r="BF1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BF1" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="BG1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BH1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="BH1" s="16" t="s">
-        <v>140</v>
-      </c>
       <c r="BI1" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BJ1" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BK1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="BM1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="BL1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="BM1" s="16" t="s">
-        <v>148</v>
-      </c>
       <c r="BN1" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BO1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="BP1" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="BP1" s="16" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.3">
@@ -1770,13 +1767,13 @@
         <v>62</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -1815,13 +1812,13 @@
         <v>76</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="Y2" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="Z2" s="13" t="s">
         <v>87</v>
@@ -1860,19 +1857,19 @@
         <v>66</v>
       </c>
       <c r="AL2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AM2" s="13" t="s">
         <v>68</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AO2" s="4" t="s">
         <v>111</v>
       </c>
       <c r="AP2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AQ2" s="2" t="s">
         <v>116</v>
@@ -1887,13 +1884,13 @@
         <v>119</v>
       </c>
       <c r="AU2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AV2" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="AW2" s="2" t="s">
-        <v>87</v>
+        <v>174</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>127</v>
@@ -1902,55 +1899,55 @@
         <v>125</v>
       </c>
       <c r="AZ2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BD2" s="2" t="s">
         <v>117</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG2" s="2" t="s">
         <v>127</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BJ2" s="2" t="s">
         <v>106</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BO2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="BP2" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1967,10 +1964,13 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -1980,28 +1980,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2012,22 +2012,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -2056,10 +2056,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2082,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6B23FB-F06E-4C7D-A14C-C7F88539098D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2096,61 +2096,61 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>117</v>
@@ -2168,7 +2168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D83E6DB-5A04-4CE4-AB6C-9127F09B31CE}">
   <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2336,52 +2336,52 @@
         <v>126</v>
       </c>
       <c r="BA1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="BB1" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="BC1" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BD1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BE1" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="BE1" s="16" t="s">
+      <c r="BF1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BF1" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="BG1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BH1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="BH1" s="16" t="s">
-        <v>140</v>
-      </c>
       <c r="BI1" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BJ1" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BK1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="BM1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="BL1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="BM1" s="16" t="s">
-        <v>148</v>
-      </c>
       <c r="BN1" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BO1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="BP1" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="BP1" s="16" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.3">
@@ -2405,13 +2405,13 @@
         <v>62</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -2450,13 +2450,13 @@
         <v>76</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Z2" s="13" t="s">
         <v>87</v>
@@ -2495,19 +2495,19 @@
         <v>66</v>
       </c>
       <c r="AL2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AM2" s="13" t="s">
         <v>68</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AO2" s="4" t="s">
         <v>111</v>
       </c>
       <c r="AP2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AQ2" s="2" t="s">
         <v>116</v>
@@ -2522,13 +2522,13 @@
         <v>119</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>127</v>
@@ -2537,55 +2537,55 @@
         <v>125</v>
       </c>
       <c r="AZ2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BD2" s="2" t="s">
         <v>117</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG2" s="2" t="s">
         <v>127</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BJ2" s="2" t="s">
         <v>106</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BO2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="BP2" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code changes done on order confirmation pages
</commit_message>
<xml_diff>
--- a/DCPLProjectSales/src/test/resources/TestData/TestData.xlsx
+++ b/DCPLProjectSales/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectSales\DCPLProjectSales\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E2598D-705B-4CB4-9308-437A6B188ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F934DCA-E15E-49F3-B32E-A2DC42712BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesLogin" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="178">
   <si>
     <t>hrms_id</t>
   </si>
@@ -561,13 +561,19 @@
   </si>
   <si>
     <t>18</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +609,12 @@
       <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -714,7 +726,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -740,6 +752,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1961,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDBC5E9-01B9-4A17-8E18-82575898BD8D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,33 +2025,40 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>128</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
         <v>117</v>
       </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L17" s="19"/>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L20" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{129DB296-04C0-4141-B533-E5D5D6FBB2BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2082,7 +2102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6B23FB-F06E-4C7D-A14C-C7F88539098D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -2168,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D83E6DB-5A04-4CE4-AB6C-9127F09B31CE}">
   <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2405,13 +2425,13 @@
         <v>62</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>128</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -2450,13 +2470,13 @@
         <v>76</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>128</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="Z2" s="13" t="s">
         <v>87</v>
@@ -2522,13 +2542,13 @@
         <v>119</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AV2" s="2" t="s">
         <v>128</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>127</v>

</xml_diff>